<commit_message>
Added feature for CSV test data, test data selection Yes/No
</commit_message>
<xml_diff>
--- a/SeleniumPractise/src/CleartripTestData.xlsx
+++ b/SeleniumPractise/src/CleartripTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13650" windowHeight="3660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13275" windowHeight="4020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="B1:G10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Onward Journey date in DD/MM/YYYY</t>
   </si>
@@ -79,9 +78,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>10/09/2020</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -112,27 +108,9 @@
     <t>Mandarmoni</t>
   </si>
   <si>
-    <t>01/02/2020</t>
-  </si>
-  <si>
-    <t>05/02/2020</t>
-  </si>
-  <si>
-    <t>08/08/2020</t>
-  </si>
-  <si>
     <t>12/02/2020</t>
   </si>
   <si>
-    <t>31/12/2019</t>
-  </si>
-  <si>
-    <t>05/01/2020</t>
-  </si>
-  <si>
-    <t>Patna</t>
-  </si>
-  <si>
     <t>Hyderabad</t>
   </si>
   <si>
@@ -142,13 +120,43 @@
     <t>Bhopal</t>
   </si>
   <si>
-    <t>29/12/2019</t>
-  </si>
-  <si>
-    <t>15/01/2020</t>
-  </si>
-  <si>
-    <t>02/02/2020</t>
+    <t>04/04/2020</t>
+  </si>
+  <si>
+    <t>01/05/2020</t>
+  </si>
+  <si>
+    <t>15/02/2020</t>
+  </si>
+  <si>
+    <t>02/03/2020</t>
+  </si>
+  <si>
+    <t>25/03/2020</t>
+  </si>
+  <si>
+    <t>05/04/2020</t>
+  </si>
+  <si>
+    <t>05/12/2020</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Bagdogra</t>
+  </si>
+  <si>
+    <t>01/06/2020</t>
+  </si>
+  <si>
+    <t>To be executed</t>
   </si>
 </sst>
 </file>
@@ -492,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
@@ -508,9 +516,10 @@
     <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
@@ -532,19 +541,22 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:8">
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
@@ -555,16 +567,19 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:8">
+      <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -578,13 +593,16 @@
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="I3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -601,8 +619,11 @@
       <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="I4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -610,10 +631,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
@@ -624,96 +645,139 @@
       <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+      <formula1>$A$8:$A$9</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" hidden="1" customWidth="1"/>
     <col min="2" max="5" width="20.28515625" style="3"/>
     <col min="6" max="6" width="20.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>$A$3:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>$A$6:$A$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -725,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes for test data dropdown modifeid
</commit_message>
<xml_diff>
--- a/SeleniumPractise/src/CleartripTestData.xlsx
+++ b/SeleniumPractise/src/CleartripTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13275" windowHeight="4020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Onward Journey date in DD/MM/YYYY</t>
   </si>
@@ -500,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
@@ -568,10 +568,13 @@
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -594,10 +597,13 @@
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -620,7 +626,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -649,20 +655,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
-      <formula1>$A$8:$A$9</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
+      <formula1>$A$3:$A$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -673,15 +669,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="2" max="5" width="20.28515625" style="3"/>
-    <col min="6" max="6" width="20.28515625" style="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="5" width="17" style="3"/>
+    <col min="6" max="6" width="17" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -787,17 +783,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A16:A17"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bug fixes and code tuning
</commit_message>
<xml_diff>
--- a/SeleniumPractise/src/CleartripTestData.xlsx
+++ b/SeleniumPractise/src/CleartripTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6345"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14910" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>09/04/2020</t>
   </si>
   <si>
-    <t>04/05/2020</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>25/03/2020</t>
   </si>
   <si>
-    <t>05/04/2020</t>
-  </si>
-  <si>
     <t>05/12/2020</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>To be executed</t>
+  </si>
+  <si>
+    <t>04/05/2021</t>
+  </si>
+  <si>
+    <t>05/04/2021</t>
   </si>
 </sst>
 </file>
@@ -500,23 +500,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:CB5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="26.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="40" width="0.140625" customWidth="1"/>
+    <col min="68" max="68" width="7.140625" customWidth="1"/>
+    <col min="69" max="69" width="8.28515625" customWidth="1"/>
+    <col min="70" max="70" width="9.7109375" customWidth="1"/>
+    <col min="71" max="71" width="5.42578125" customWidth="1"/>
+    <col min="72" max="72" width="15" customWidth="1"/>
+    <col min="73" max="73" width="17.42578125" customWidth="1"/>
+    <col min="74" max="74" width="21.5703125" customWidth="1"/>
+    <col min="75" max="75" width="10" customWidth="1"/>
+    <col min="80" max="80" width="18.7109375" customWidth="1"/>
+    <col min="103" max="103" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -542,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -550,42 +561,42 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -597,24 +608,24 @@
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -623,36 +634,36 @@
         <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +681,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -682,89 +693,89 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -796,12 +807,12 @@
   <sheetData>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>